<commit_message>
Some changes i don't remember it was like a year ago
</commit_message>
<xml_diff>
--- a/Experimental Results Table.xlsx
+++ b/Experimental Results Table.xlsx
@@ -384,12 +384,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>18</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -399,12 +399,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>19</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -414,12 +414,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>24</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>13</t>
         </is>
       </c>
     </row>
@@ -429,12 +429,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -444,12 +444,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>22</t>
         </is>
       </c>
     </row>
@@ -459,12 +459,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>4</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>9</t>
         </is>
       </c>
     </row>
@@ -474,12 +474,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>22</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>6</t>
         </is>
       </c>
     </row>
@@ -489,12 +489,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
           <t>1</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>5</t>
         </is>
       </c>
     </row>
@@ -504,12 +504,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>11</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -519,12 +519,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>24</t>
         </is>
       </c>
     </row>

</xml_diff>